<commit_message>
fix double entrys for 2023-05-16 in BL and LK
</commit_message>
<xml_diff>
--- a/dataStore/frozen-incidence/BL.xlsx
+++ b/dataStore/frozen-incidence/BL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="39">
   <si>
     <t>Datenstand</t>
   </si>
@@ -492,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E528"/>
+  <dimension ref="A1:E511"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8629,16 +8629,16 @@
         <v>45062</v>
       </c>
       <c r="B479" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C479" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D479">
-        <v>5486</v>
+        <v>344</v>
       </c>
       <c r="E479">
-        <v>6.590809168274483</v>
+        <v>11.77273823966763</v>
       </c>
     </row>
     <row r="480" spans="1:5">
@@ -8646,16 +8646,16 @@
         <v>45062</v>
       </c>
       <c r="B480" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C480" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D480">
-        <v>344</v>
+        <v>198</v>
       </c>
       <c r="E480">
-        <v>11.77273823966763</v>
+        <v>10.6799860836545</v>
       </c>
     </row>
     <row r="481" spans="1:5">
@@ -8663,16 +8663,16 @@
         <v>45062</v>
       </c>
       <c r="B481" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C481" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D481">
-        <v>344</v>
+        <v>638</v>
       </c>
       <c r="E481">
-        <v>11.77273823966763</v>
+        <v>7.948144214218185</v>
       </c>
     </row>
     <row r="482" spans="1:5">
@@ -8680,16 +8680,16 @@
         <v>45062</v>
       </c>
       <c r="B482" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C482" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D482">
-        <v>198</v>
+        <v>25</v>
       </c>
       <c r="E482">
-        <v>10.6799860836545</v>
+        <v>3.695693629954631</v>
       </c>
     </row>
     <row r="483" spans="1:5">
@@ -8697,16 +8697,16 @@
         <v>45062</v>
       </c>
       <c r="B483" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C483" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D483">
-        <v>198</v>
+        <v>1025</v>
       </c>
       <c r="E483">
-        <v>10.6799860836545</v>
+        <v>5.718401050266642</v>
       </c>
     </row>
     <row r="484" spans="1:5">
@@ -8714,16 +8714,16 @@
         <v>45062</v>
       </c>
       <c r="B484" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C484" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D484">
-        <v>638</v>
+        <v>386</v>
       </c>
       <c r="E484">
-        <v>7.948144214218185</v>
+        <v>6.131834115777606</v>
       </c>
     </row>
     <row r="485" spans="1:5">
@@ -8731,16 +8731,16 @@
         <v>45062</v>
       </c>
       <c r="B485" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C485" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D485">
-        <v>638</v>
+        <v>190</v>
       </c>
       <c r="E485">
-        <v>7.948144214218185</v>
+        <v>4.626828053676076</v>
       </c>
     </row>
     <row r="486" spans="1:5">
@@ -8748,16 +8748,16 @@
         <v>45062</v>
       </c>
       <c r="B486" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C486" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D486">
-        <v>25</v>
+        <v>431</v>
       </c>
       <c r="E486">
-        <v>3.695693629954632</v>
+        <v>3.874281976894178</v>
       </c>
     </row>
     <row r="487" spans="1:5">
@@ -8765,16 +8765,16 @@
         <v>45062</v>
       </c>
       <c r="B487" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C487" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D487">
-        <v>25</v>
+        <v>690</v>
       </c>
       <c r="E487">
-        <v>3.695693629954632</v>
+        <v>5.236401123200451</v>
       </c>
     </row>
     <row r="488" spans="1:5">
@@ -8782,16 +8782,16 @@
         <v>45062</v>
       </c>
       <c r="B488" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C488" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D488">
-        <v>1025</v>
+        <v>88</v>
       </c>
       <c r="E488">
-        <v>5.718401050266642</v>
+        <v>8.958128891187236</v>
       </c>
     </row>
     <row r="489" spans="1:5">
@@ -8799,16 +8799,16 @@
         <v>45062</v>
       </c>
       <c r="B489" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C489" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D489">
-        <v>1025</v>
+        <v>373</v>
       </c>
       <c r="E489">
-        <v>5.718401050266642</v>
+        <v>10.14283725341756</v>
       </c>
     </row>
     <row r="490" spans="1:5">
@@ -8816,16 +8816,16 @@
         <v>45062</v>
       </c>
       <c r="B490" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C490" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D490">
-        <v>386</v>
+        <v>249</v>
       </c>
       <c r="E490">
-        <v>6.131834115777606</v>
+        <v>9.811384989290223</v>
       </c>
     </row>
     <row r="491" spans="1:5">
@@ -8833,16 +8833,16 @@
         <v>45062</v>
       </c>
       <c r="B491" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C491" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D491">
-        <v>386</v>
+        <v>223</v>
       </c>
       <c r="E491">
-        <v>6.131834115777606</v>
+        <v>13.84095930882097</v>
       </c>
     </row>
     <row r="492" spans="1:5">
@@ -8850,16 +8850,16 @@
         <v>45062</v>
       </c>
       <c r="B492" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C492" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D492">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="E492">
-        <v>4.626828053676076</v>
+        <v>5.837246679571269</v>
       </c>
     </row>
     <row r="493" spans="1:5">
@@ -8867,16 +8867,16 @@
         <v>45062</v>
       </c>
       <c r="B493" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C493" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D493">
-        <v>190</v>
+        <v>253</v>
       </c>
       <c r="E493">
-        <v>4.626828053676076</v>
+        <v>11.66300104229428</v>
       </c>
     </row>
     <row r="494" spans="1:5">
@@ -8884,293 +8884,293 @@
         <v>45062</v>
       </c>
       <c r="B494" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C494" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D494">
-        <v>431</v>
+        <v>137</v>
       </c>
       <c r="E494">
-        <v>3.874281976894178</v>
+        <v>6.496391657495058</v>
       </c>
     </row>
     <row r="495" spans="1:5">
       <c r="A495" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B495" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C495" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D495">
-        <v>431</v>
+        <v>5185</v>
       </c>
       <c r="E495">
-        <v>3.874281976894178</v>
+        <v>6.229191676540867</v>
       </c>
     </row>
     <row r="496" spans="1:5">
       <c r="A496" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B496" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C496" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D496">
-        <v>690</v>
+        <v>292</v>
       </c>
       <c r="E496">
-        <v>5.236401123200452</v>
+        <v>9.993138273206242</v>
       </c>
     </row>
     <row r="497" spans="1:5">
       <c r="A497" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B497" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C497" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D497">
-        <v>690</v>
+        <v>192</v>
       </c>
       <c r="E497">
-        <v>5.236401123200452</v>
+        <v>10.35635014172557</v>
       </c>
     </row>
     <row r="498" spans="1:5">
       <c r="A498" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B498" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C498" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D498">
-        <v>88</v>
+        <v>638</v>
       </c>
       <c r="E498">
-        <v>8.958128891187236</v>
+        <v>7.948144214218185</v>
       </c>
     </row>
     <row r="499" spans="1:5">
       <c r="A499" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B499" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C499" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D499">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="E499">
-        <v>8.958128891187236</v>
+        <v>2.80872715876552</v>
       </c>
     </row>
     <row r="500" spans="1:5">
       <c r="A500" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B500" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C500" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D500">
-        <v>373</v>
+        <v>904</v>
       </c>
       <c r="E500">
-        <v>10.14283725341756</v>
+        <v>5.043350779942482</v>
       </c>
     </row>
     <row r="501" spans="1:5">
       <c r="A501" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B501" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C501" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D501">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="E501">
-        <v>10.14283725341756</v>
+        <v>5.734694600507035</v>
       </c>
     </row>
     <row r="502" spans="1:5">
       <c r="A502" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B502" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C502" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D502">
-        <v>249</v>
+        <v>184</v>
       </c>
       <c r="E502">
-        <v>9.811384989290223</v>
+        <v>4.480717694086305</v>
       </c>
     </row>
     <row r="503" spans="1:5">
       <c r="A503" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B503" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C503" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D503">
-        <v>249</v>
+        <v>406</v>
       </c>
       <c r="E503">
-        <v>9.811384989290223</v>
+        <v>3.649555644127694</v>
       </c>
     </row>
     <row r="504" spans="1:5">
       <c r="A504" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B504" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C504" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D504">
-        <v>223</v>
+        <v>679</v>
       </c>
       <c r="E504">
-        <v>13.84095930882097</v>
+        <v>5.152922264714648</v>
       </c>
     </row>
     <row r="505" spans="1:5">
       <c r="A505" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B505" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C505" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D505">
-        <v>223</v>
+        <v>85</v>
       </c>
       <c r="E505">
-        <v>13.84095930882097</v>
+        <v>8.652738133533127</v>
       </c>
     </row>
     <row r="506" spans="1:5">
       <c r="A506" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B506" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C506" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D506">
-        <v>236</v>
+        <v>346</v>
       </c>
       <c r="E506">
-        <v>5.837246679571269</v>
+        <v>9.408637237754631</v>
       </c>
     </row>
     <row r="507" spans="1:5">
       <c r="A507" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B507" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C507" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D507">
-        <v>236</v>
+        <v>210</v>
       </c>
       <c r="E507">
-        <v>5.837246679571269</v>
+        <v>8.274662039160429</v>
       </c>
     </row>
     <row r="508" spans="1:5">
       <c r="A508" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B508" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C508" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D508">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="E508">
-        <v>11.66300104229428</v>
+        <v>13.90302639092331</v>
       </c>
     </row>
     <row r="509" spans="1:5">
       <c r="A509" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B509" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C509" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D509">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="E509">
-        <v>11.66300104229428</v>
+        <v>6.505067274267982</v>
       </c>
     </row>
     <row r="510" spans="1:5">
       <c r="A510" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B510" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C510" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D510">
-        <v>137</v>
+        <v>239</v>
       </c>
       <c r="E510">
-        <v>6.496391657495058</v>
+        <v>11.01761758540843</v>
       </c>
     </row>
     <row r="511" spans="1:5">
       <c r="A511" s="2">
-        <v>45062</v>
+        <v>45063</v>
       </c>
       <c r="B511" t="s">
         <v>21</v>
@@ -9179,298 +9179,9 @@
         <v>38</v>
       </c>
       <c r="D511">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E511">
-        <v>6.496391657495058</v>
-      </c>
-    </row>
-    <row r="512" spans="1:5">
-      <c r="A512" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B512" t="s">
-        <v>5</v>
-      </c>
-      <c r="C512" t="s">
-        <v>22</v>
-      </c>
-      <c r="D512">
-        <v>5185</v>
-      </c>
-      <c r="E512">
-        <v>6.229191676540867</v>
-      </c>
-    </row>
-    <row r="513" spans="1:5">
-      <c r="A513" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B513" t="s">
-        <v>6</v>
-      </c>
-      <c r="C513" t="s">
-        <v>23</v>
-      </c>
-      <c r="D513">
-        <v>292</v>
-      </c>
-      <c r="E513">
-        <v>9.993138273206242</v>
-      </c>
-    </row>
-    <row r="514" spans="1:5">
-      <c r="A514" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B514" t="s">
-        <v>7</v>
-      </c>
-      <c r="C514" t="s">
-        <v>24</v>
-      </c>
-      <c r="D514">
-        <v>192</v>
-      </c>
-      <c r="E514">
-        <v>10.35635014172557</v>
-      </c>
-    </row>
-    <row r="515" spans="1:5">
-      <c r="A515" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B515" t="s">
-        <v>8</v>
-      </c>
-      <c r="C515" t="s">
-        <v>25</v>
-      </c>
-      <c r="D515">
-        <v>638</v>
-      </c>
-      <c r="E515">
-        <v>7.948144214218185</v>
-      </c>
-    </row>
-    <row r="516" spans="1:5">
-      <c r="A516" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B516" t="s">
-        <v>9</v>
-      </c>
-      <c r="C516" t="s">
-        <v>26</v>
-      </c>
-      <c r="D516">
-        <v>19</v>
-      </c>
-      <c r="E516">
-        <v>2.80872715876552</v>
-      </c>
-    </row>
-    <row r="517" spans="1:5">
-      <c r="A517" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B517" t="s">
-        <v>10</v>
-      </c>
-      <c r="C517" t="s">
-        <v>27</v>
-      </c>
-      <c r="D517">
-        <v>904</v>
-      </c>
-      <c r="E517">
-        <v>5.043350779942482</v>
-      </c>
-    </row>
-    <row r="518" spans="1:5">
-      <c r="A518" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B518" t="s">
-        <v>11</v>
-      </c>
-      <c r="C518" t="s">
-        <v>28</v>
-      </c>
-      <c r="D518">
-        <v>361</v>
-      </c>
-      <c r="E518">
-        <v>5.734694600507035</v>
-      </c>
-    </row>
-    <row r="519" spans="1:5">
-      <c r="A519" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B519" t="s">
-        <v>12</v>
-      </c>
-      <c r="C519" t="s">
-        <v>29</v>
-      </c>
-      <c r="D519">
-        <v>184</v>
-      </c>
-      <c r="E519">
-        <v>4.480717694086305</v>
-      </c>
-    </row>
-    <row r="520" spans="1:5">
-      <c r="A520" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B520" t="s">
-        <v>13</v>
-      </c>
-      <c r="C520" t="s">
-        <v>30</v>
-      </c>
-      <c r="D520">
-        <v>406</v>
-      </c>
-      <c r="E520">
-        <v>3.649555644127694</v>
-      </c>
-    </row>
-    <row r="521" spans="1:5">
-      <c r="A521" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B521" t="s">
-        <v>14</v>
-      </c>
-      <c r="C521" t="s">
-        <v>31</v>
-      </c>
-      <c r="D521">
-        <v>679</v>
-      </c>
-      <c r="E521">
-        <v>5.152922264714648</v>
-      </c>
-    </row>
-    <row r="522" spans="1:5">
-      <c r="A522" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B522" t="s">
-        <v>15</v>
-      </c>
-      <c r="C522" t="s">
-        <v>32</v>
-      </c>
-      <c r="D522">
-        <v>85</v>
-      </c>
-      <c r="E522">
-        <v>8.652738133533127</v>
-      </c>
-    </row>
-    <row r="523" spans="1:5">
-      <c r="A523" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B523" t="s">
-        <v>16</v>
-      </c>
-      <c r="C523" t="s">
-        <v>33</v>
-      </c>
-      <c r="D523">
-        <v>346</v>
-      </c>
-      <c r="E523">
-        <v>9.408637237754631</v>
-      </c>
-    </row>
-    <row r="524" spans="1:5">
-      <c r="A524" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B524" t="s">
-        <v>17</v>
-      </c>
-      <c r="C524" t="s">
-        <v>34</v>
-      </c>
-      <c r="D524">
-        <v>210</v>
-      </c>
-      <c r="E524">
-        <v>8.274662039160429</v>
-      </c>
-    </row>
-    <row r="525" spans="1:5">
-      <c r="A525" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B525" t="s">
-        <v>18</v>
-      </c>
-      <c r="C525" t="s">
-        <v>35</v>
-      </c>
-      <c r="D525">
-        <v>224</v>
-      </c>
-      <c r="E525">
-        <v>13.90302639092331</v>
-      </c>
-    </row>
-    <row r="526" spans="1:5">
-      <c r="A526" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B526" t="s">
-        <v>19</v>
-      </c>
-      <c r="C526" t="s">
-        <v>36</v>
-      </c>
-      <c r="D526">
-        <v>263</v>
-      </c>
-      <c r="E526">
-        <v>6.505067274267982</v>
-      </c>
-    </row>
-    <row r="527" spans="1:5">
-      <c r="A527" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B527" t="s">
-        <v>20</v>
-      </c>
-      <c r="C527" t="s">
-        <v>37</v>
-      </c>
-      <c r="D527">
-        <v>239</v>
-      </c>
-      <c r="E527">
-        <v>11.01761758540843</v>
-      </c>
-    </row>
-    <row r="528" spans="1:5">
-      <c r="A528" s="2">
-        <v>45063</v>
-      </c>
-      <c r="B528" t="s">
-        <v>21</v>
-      </c>
-      <c r="C528" t="s">
-        <v>38</v>
-      </c>
-      <c r="D528">
-        <v>143</v>
-      </c>
-      <c r="E528">
         <v>6.780905160743016</v>
       </c>
     </row>

</xml_diff>